<commit_message>
Uradjeni fajlovi za budzet
TODO: Matrica + mali fajl
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACKUP_20012013_MyDoc\NASTAVA\SI3USP - Upravljanje softverskim projektima\Projekat\Projekat 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fax\USPprojekat\USP-projekat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A952EB-C74D-426A-BE4F-19E3275312A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A4F9E4-3E56-4D17-8841-A7BC222548DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Equipment - budzet" sheetId="3" r:id="rId3"/>
     <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Equipment - budzet'!$B$4:$I$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -67,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="100">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -195,33 +198,6 @@
     <t>[ If yes, please describe the third party and their contributions]</t>
   </si>
   <si>
-    <t>WP1-</t>
-  </si>
-  <si>
-    <t>WP2-</t>
-  </si>
-  <si>
-    <t>WP3-</t>
-  </si>
-  <si>
-    <t>WP4-</t>
-  </si>
-  <si>
-    <t>WP5-</t>
-  </si>
-  <si>
-    <t>WP6-</t>
-  </si>
-  <si>
-    <t>WP7-</t>
-  </si>
-  <si>
-    <t>WP8-</t>
-  </si>
-  <si>
-    <t>WP9-</t>
-  </si>
-  <si>
     <t>WP10-</t>
   </si>
   <si>
@@ -283,6 +259,117 @@
   </si>
   <si>
     <t>Experts</t>
+  </si>
+  <si>
+    <t>WP1</t>
+  </si>
+  <si>
+    <t>WP4</t>
+  </si>
+  <si>
+    <t>TOM</t>
+  </si>
+  <si>
+    <t>"TomTom N.V."</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Amsterdam, NL</t>
+  </si>
+  <si>
+    <t>Belgrade, SRB</t>
+  </si>
+  <si>
+    <t>GOOGLE</t>
+  </si>
+  <si>
+    <t>"Google Spain, S.L."</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Madrid, ESP</t>
+  </si>
+  <si>
+    <t>WP5</t>
+  </si>
+  <si>
+    <t>MSG</t>
+  </si>
+  <si>
+    <t>"Message Bird"</t>
+  </si>
+  <si>
+    <t>WP6</t>
+  </si>
+  <si>
+    <t>TEL</t>
+  </si>
+  <si>
+    <t>Telekom Srbija</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Computer Server, 3.5GHz CPU, 32GB RAM, 2x500GB SSD</t>
+  </si>
+  <si>
+    <t>Network Modem, 1GBPs, good range, compatible with DSL technologies</t>
+  </si>
+  <si>
+    <t>Desktop-PC, 3GHz CPU, Octa-core, 16GB RAM, 512GB SSD</t>
+  </si>
+  <si>
+    <t>License acquiring, administrative and legal duties, necessary for "Google Play" and "Google Maps"</t>
+  </si>
+  <si>
+    <t>License acquiring, administrative and legal duties, necessary for using "TomTom Maps"</t>
+  </si>
+  <si>
+    <t>ETF</t>
+  </si>
+  <si>
+    <t>School of Electrical Engineering</t>
+  </si>
+  <si>
+    <t>WP1-WP9</t>
+  </si>
+  <si>
+    <t>FON</t>
+  </si>
+  <si>
+    <t>Faculty of Organizational Sciences</t>
+  </si>
+  <si>
+    <t>WP1- Upravljanje projektom</t>
+  </si>
+  <si>
+    <t>WP2- Planiranje projekta</t>
+  </si>
+  <si>
+    <t>WP3- Dizajniranje arhitekture sistema</t>
+  </si>
+  <si>
+    <t>WP4- Postavljanje neophodne infrastrukture</t>
+  </si>
+  <si>
+    <t>WP5- Razvoj veb sistema sa serverskim I klijentkim delom</t>
+  </si>
+  <si>
+    <t>WP6-  Povezivanje sa "Google Maps" i "TomTom" bazama podataka</t>
+  </si>
+  <si>
+    <t>WP7- Adaptiranje aplikacija za mobilne uredjaje (Android)</t>
+  </si>
+  <si>
+    <t>WP8- Integracija i testiranje sistema</t>
+  </si>
+  <si>
+    <t>WP9- Evaluacija I disiminacija</t>
   </si>
 </sst>
 </file>
@@ -292,7 +379,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +474,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -637,7 +730,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -737,50 +830,9 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -802,14 +854,56 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1242,89 +1336,91 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="5.54296875" customWidth="1"/>
-    <col min="6" max="6" width="5.26953125" customWidth="1"/>
-    <col min="7" max="7" width="5.1796875" customWidth="1"/>
-    <col min="8" max="8" width="5.26953125" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="13" width="14.1796875" customWidth="1"/>
-    <col min="14" max="14" width="15.1796875" customWidth="1"/>
-    <col min="15" max="19" width="14.1796875" customWidth="1"/>
+    <col min="10" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="19" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="3"/>
-      <c r="L4" s="65" t="s">
+      <c r="L4" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="3"/>
-      <c r="L5" s="65" t="s">
+      <c r="L5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="3"/>
-      <c r="L6" s="65" t="s">
+      <c r="L6" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1333,85 +1429,85 @@
       </c>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E7" s="65" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E7" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
       <c r="J7" s="3"/>
-      <c r="L7" s="65" t="s">
+      <c r="L7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J8" s="2"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="66" t="s">
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
       <c r="S10" s="8"/>
     </row>
-    <row r="12" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="D12" s="68" t="s">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69" t="s">
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="56"/>
       <c r="S12" s="9"/>
     </row>
-    <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62" t="s">
+    <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="72" t="s">
-        <v>70</v>
-      </c>
       <c r="E13" s="10" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>15</v>
@@ -1456,12 +1552,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1472,17 +1568,16 @@
         <v>0</v>
       </c>
       <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
       <c r="O14" s="18">
-        <f t="shared" ref="O14:O23" si="0">+$O$4*(J14+K14-N14)</f>
+        <f>+$O$4*(J14+K19-N14)</f>
         <v>0</v>
       </c>
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
-        <f>+J14+K14+L14+M14+O14+P14</f>
+        <f>+J14+K19+L14+M14+O14+P14</f>
         <v>0</v>
       </c>
       <c r="R14" s="18"/>
@@ -1491,19 +1586,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="16">
-        <f t="shared" ref="I15:I23" si="1">+SUM(D15:H15)</f>
+        <f t="shared" ref="I15:I23" si="0">+SUM(D15:H15)</f>
         <v>0</v>
       </c>
       <c r="J15" s="17"/>
@@ -1512,7 +1607,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="O14:O23" si="1">+$O$4*(J15+K15-N15)</f>
         <v>0</v>
       </c>
       <c r="P15" s="17"/>
@@ -1526,19 +1621,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16" s="17"/>
@@ -1547,7 +1642,7 @@
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P16" s="17"/>
@@ -1561,19 +1656,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J17" s="17"/>
@@ -1582,7 +1677,7 @@
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P17" s="17"/>
@@ -1596,19 +1691,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J18" s="17"/>
@@ -1617,7 +1712,7 @@
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P18" s="17"/>
@@ -1631,19 +1726,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J19" s="17"/>
@@ -1651,34 +1746,34 @@
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
-      <c r="O19" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="O19" s="18" t="e">
+        <f>+$O$4*(J19+#REF!-N19)</f>
+        <v>#REF!</v>
       </c>
       <c r="P19" s="17"/>
-      <c r="Q19" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="Q19" s="17" t="e">
+        <f>+J19+#REF!+L19+M19+O19+P19</f>
+        <v>#REF!</v>
       </c>
       <c r="R19" s="18"/>
-      <c r="S19" s="18">
+      <c r="S19" s="18" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J20" s="17"/>
@@ -1687,7 +1782,7 @@
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P20" s="17"/>
@@ -1701,19 +1796,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J21" s="17"/>
@@ -1722,7 +1817,7 @@
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
       <c r="O21" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P21" s="17"/>
@@ -1736,19 +1831,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J22" s="17"/>
@@ -1757,7 +1852,7 @@
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P22" s="17"/>
@@ -1771,19 +1866,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J23" s="17"/>
@@ -1792,7 +1887,7 @@
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
       <c r="O23" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P23" s="17"/>
@@ -1806,12 +1901,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" s="61" t="s">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
         <v>0</v>
@@ -1841,11 +1936,11 @@
         <v>0</v>
       </c>
       <c r="K24" s="20">
-        <f t="shared" ref="K24:S24" si="5">SUM(K14:K23)</f>
+        <f>SUM(K15:K23)</f>
         <v>0</v>
       </c>
       <c r="L24" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K24:S24" si="5">SUM(L14:L23)</f>
         <v>0</v>
       </c>
       <c r="M24" s="20">
@@ -1856,29 +1951,29 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O24" s="20">
+      <c r="O24" s="20" t="e">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="P24" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24" s="20" t="e">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="R24" s="21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S24" s="22">
+      <c r="S24" s="22" t="e">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="T24" s="23"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -1900,7 +1995,7 @@
       <c r="S25" s="23"/>
       <c r="T25" s="23"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
@@ -1927,31 +2022,31 @@
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="30"/>
       <c r="S27" s="31"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" s="60" t="s">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -1969,7 +2064,7 @@
       <c r="O29" s="32"/>
       <c r="P29" s="32"/>
     </row>
-    <row r="30" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>31</v>
       </c>
@@ -1989,99 +2084,99 @@
       <c r="O30" s="32"/>
       <c r="P30" s="32"/>
     </row>
-    <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="53" t="str">
+    <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="60" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B31" s="54"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="57" t="s">
+      <c r="D31" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-    </row>
-    <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="47" t="s">
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="62"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
+      <c r="P31" s="62"/>
+    </row>
+    <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="47"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="59" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
+      <c r="D32" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="65"/>
       <c r="S32" s="31"/>
     </row>
-    <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="47" t="s">
+    <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="47"/>
+      <c r="B33" s="63"/>
       <c r="C33" s="35"/>
-      <c r="D33" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
+      <c r="D33" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="65"/>
+      <c r="O33" s="65"/>
+      <c r="P33" s="65"/>
       <c r="S33" s="31"/>
     </row>
-    <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="47" t="s">
+    <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="47"/>
+      <c r="B34" s="63"/>
       <c r="C34" s="35"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="65"/>
+      <c r="N34" s="65"/>
+      <c r="O34" s="65"/>
+      <c r="P34" s="65"/>
       <c r="S34" s="31"/>
     </row>
-    <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="37"/>
       <c r="E35" s="37"/>
       <c r="F35" s="37"/>
@@ -2096,7 +2191,7 @@
       <c r="O35" s="37"/>
       <c r="P35" s="37"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D36" s="38"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
@@ -2111,105 +2206,133 @@
       <c r="O36" s="38"/>
       <c r="P36" s="38"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A37" s="53" t="str">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="60" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="54"/>
+      <c r="B37" s="61"/>
       <c r="C37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="55" t="s">
+      <c r="D37" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-    </row>
-    <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="47" t="s">
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
+      <c r="N37" s="71"/>
+      <c r="O37" s="71"/>
+      <c r="P37" s="71"/>
+    </row>
+    <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="47"/>
+      <c r="B38" s="63"/>
       <c r="C38" s="35"/>
-      <c r="D38" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-      <c r="L38" s="52"/>
-      <c r="M38" s="52"/>
-      <c r="N38" s="52"/>
-      <c r="O38" s="52"/>
-      <c r="P38" s="52"/>
+      <c r="D38" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="65"/>
+      <c r="O38" s="65"/>
+      <c r="P38" s="65"/>
       <c r="S38" s="31"/>
     </row>
-    <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="47" t="s">
+    <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="47"/>
+      <c r="B39" s="63"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="50"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="67"/>
+      <c r="P39" s="68"/>
       <c r="S39" s="31"/>
     </row>
-    <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="47" t="s">
+    <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="47"/>
+      <c r="B40" s="63"/>
       <c r="C40" s="35"/>
-      <c r="D40" s="51" t="s">
+      <c r="D40" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="65"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="65"/>
+      <c r="M40" s="65"/>
+      <c r="N40" s="65"/>
+      <c r="O40" s="65"/>
+      <c r="P40" s="65"/>
       <c r="S40" s="31"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="J14:N23 C32:P40 D14:H23 P14:P23 R14:S23 O6" name="Range1"/>
+    <protectedRange sqref="C32:P40 D14:H23 P14:P23 R14:S23 O6 J14:J23 L14:N23 K15:K23" name="Range1"/>
   </protectedRanges>
   <mergeCells count="41">
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:P39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:P40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:P34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E4:I4"/>
@@ -2223,34 +2346,6 @@
     <mergeCell ref="A10:R10"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="J12:R12"/>
-    <mergeCell ref="A28:P28"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:P39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:P40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -2273,45 +2368,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:16" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="71"/>
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="73"/>
       <c r="D2" s="43">
         <f>SUM(P5:P35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="162" x14ac:dyDescent="0.35">
+        <v>133360</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B4" s="41" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C4" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="G4" s="44" t="s">
         <v>54</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>63</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>13</v>
@@ -2329,179 +2427,363 @@
         <v>17</v>
       </c>
       <c r="M4" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="C5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="D5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="E5" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="39">
+        <v>4</v>
+      </c>
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
+      <c r="M5" s="39">
+        <v>4</v>
+      </c>
+      <c r="N5" s="39">
+        <v>3200</v>
+      </c>
+      <c r="O5" s="39">
+        <v>960</v>
+      </c>
       <c r="P5" s="39">
         <f>N5+O5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+        <v>4160</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="39">
+        <v>4</v>
+      </c>
       <c r="I6" s="39"/>
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
       <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
+      <c r="M6" s="39">
+        <v>4</v>
+      </c>
+      <c r="N6" s="39">
+        <v>4000</v>
+      </c>
+      <c r="O6" s="39">
+        <v>960</v>
+      </c>
       <c r="P6" s="39">
         <f t="shared" ref="P6:P35" si="0">N6+O6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="39">
+        <v>8</v>
+      </c>
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
       <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
+      <c r="M7" s="39">
+        <v>14</v>
+      </c>
+      <c r="N7" s="39">
+        <v>6400</v>
+      </c>
+      <c r="O7" s="39">
+        <v>8320</v>
+      </c>
       <c r="P7" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+        <v>14720</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="39">
+        <v>8</v>
+      </c>
       <c r="I8" s="39"/>
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
       <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
+      <c r="M8" s="39">
+        <v>20</v>
+      </c>
+      <c r="N8" s="39">
+        <v>6400</v>
+      </c>
+      <c r="O8" s="39">
+        <v>12160</v>
+      </c>
       <c r="P8" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+        <v>18560</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="39">
+        <v>8</v>
+      </c>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
       <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
+      <c r="M9" s="39">
+        <v>20</v>
+      </c>
+      <c r="N9" s="39">
+        <v>8000</v>
+      </c>
+      <c r="O9" s="39">
+        <v>12160</v>
+      </c>
       <c r="P9" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
+        <v>20160</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="39">
+        <v>5</v>
+      </c>
+      <c r="I10" s="39">
+        <v>2</v>
+      </c>
+      <c r="J10" s="39">
+        <v>2</v>
+      </c>
+      <c r="K10" s="39">
+        <v>2</v>
+      </c>
+      <c r="L10" s="39">
+        <v>1</v>
+      </c>
+      <c r="M10" s="39">
+        <v>7</v>
+      </c>
+      <c r="N10" s="39">
+        <v>9600</v>
+      </c>
+      <c r="O10" s="39">
+        <v>14400</v>
+      </c>
       <c r="P10" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="47">
+        <v>5</v>
+      </c>
+      <c r="I11" s="47">
+        <v>2</v>
+      </c>
+      <c r="J11" s="47">
+        <v>2</v>
+      </c>
+      <c r="K11" s="47">
+        <v>2</v>
+      </c>
+      <c r="L11" s="47">
+        <v>1</v>
+      </c>
+      <c r="M11" s="47">
+        <v>7</v>
+      </c>
+      <c r="N11" s="47">
+        <v>12000</v>
+      </c>
+      <c r="O11" s="47">
+        <v>10800</v>
+      </c>
       <c r="P11" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
+        <v>22800</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="47">
+        <v>5</v>
+      </c>
+      <c r="I12" s="47">
+        <v>2</v>
+      </c>
+      <c r="J12" s="47">
+        <v>2</v>
+      </c>
+      <c r="K12" s="47">
+        <v>2</v>
+      </c>
+      <c r="L12" s="47">
+        <v>1</v>
+      </c>
+      <c r="M12" s="47">
+        <v>7</v>
+      </c>
+      <c r="N12" s="47">
+        <v>9600</v>
+      </c>
+      <c r="O12" s="47">
+        <v>14400</v>
+      </c>
       <c r="P12" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -2521,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -2541,7 +2823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -2561,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -2581,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -2601,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
@@ -2621,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -2641,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="39"/>
@@ -2661,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
       <c r="D21" s="39"/>
@@ -2681,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -2701,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
@@ -2721,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
       <c r="D24" s="39"/>
@@ -2741,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -2761,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
@@ -2781,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
@@ -2801,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
       <c r="D28" s="39"/>
@@ -2821,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
@@ -2841,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
@@ -2861,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
@@ -2881,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
@@ -2901,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
@@ -2921,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
@@ -2941,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>
@@ -2965,6 +3247,7 @@
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2973,174 +3256,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="6" max="6" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="66.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="71"/>
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="73"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>111804</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="41" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="39">
+        <v>2000</v>
+      </c>
+      <c r="H5" s="39">
+        <v>6</v>
+      </c>
       <c r="I5" s="39">
         <f>G5*H5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="39">
+        <v>100</v>
+      </c>
+      <c r="H6" s="39">
+        <v>10</v>
+      </c>
       <c r="I6" s="39">
         <f t="shared" ref="I6:I35" si="0">G6*H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="39">
+        <v>1300</v>
+      </c>
+      <c r="H7" s="39">
+        <v>2</v>
+      </c>
       <c r="I7" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="47">
+        <v>1300</v>
+      </c>
+      <c r="H8" s="39">
+        <v>2</v>
+      </c>
       <c r="I8" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="47">
+        <v>1300</v>
+      </c>
+      <c r="H9" s="39">
+        <v>4</v>
+      </c>
       <c r="I9" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="47">
+        <v>1300</v>
+      </c>
+      <c r="H10" s="39">
+        <v>4</v>
+      </c>
       <c r="I10" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="47">
+        <v>1301</v>
+      </c>
+      <c r="H11" s="39">
+        <v>4</v>
+      </c>
       <c r="I11" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+        <v>5204</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="39">
+        <v>1300</v>
+      </c>
+      <c r="H12" s="39">
+        <v>50</v>
+      </c>
       <c r="I12" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="39">
+        <v>1300</v>
+      </c>
+      <c r="H13" s="39">
+        <v>10</v>
+      </c>
       <c r="I13" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -3153,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -3166,7 +3577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -3179,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -3192,7 +3603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
@@ -3205,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -3218,7 +3629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="39"/>
@@ -3231,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
       <c r="D21" s="39"/>
@@ -3244,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -3257,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
@@ -3270,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
       <c r="D24" s="39"/>
@@ -3283,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -3296,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
@@ -3309,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
@@ -3322,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
       <c r="D28" s="39"/>
@@ -3335,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
@@ -3348,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
@@ -3361,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
@@ -3374,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
@@ -3387,7 +3798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
@@ -3400,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
@@ -3413,7 +3824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>
@@ -3430,6 +3841,7 @@
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3439,82 +3851,111 @@
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="6" max="6" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="87" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="71"/>
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="73"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="41" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="39">
+        <v>3000</v>
+      </c>
+      <c r="H5" s="39">
+        <v>1</v>
+      </c>
       <c r="I5" s="39">
         <f>G5*H5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="39">
+        <v>2000</v>
+      </c>
+      <c r="H6" s="39">
+        <v>1</v>
+      </c>
       <c r="I6" s="39">
         <f t="shared" ref="I6:I35" si="0">G6*H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -3527,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -3540,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -3553,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -3566,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -3579,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -3592,7 +4033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -3605,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -3618,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -3631,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -3644,7 +4085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -3657,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
@@ -3670,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -3683,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="39"/>
@@ -3696,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
       <c r="D21" s="39"/>
@@ -3709,7 +4150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -3722,7 +4163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
@@ -3735,7 +4176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
       <c r="D24" s="39"/>
@@ -3748,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -3761,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
@@ -3774,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
@@ -3787,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
       <c r="D28" s="39"/>
@@ -3800,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
@@ -3813,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
@@ -3826,7 +4267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
@@ -3839,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
@@ -3852,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
@@ -3865,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
@@ -3878,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>

</xml_diff>

<commit_message>
Uradjeno sveee, dodate dve tabele partnera i prez
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Local_Git_Repos\ProjekatUSP\ValerijanBranch\USP-projekat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Local_Git_Repos\ProjekatUSP\USP-projekat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,11 +14,11 @@
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
     <sheet name="Travel - budzet" sheetId="2" r:id="rId2"/>
-    <sheet name="Equipment - budzet" sheetId="3" r:id="rId3"/>
-    <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId4"/>
+    <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId3"/>
+    <sheet name="Equipment - budzet" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Equipment - budzet'!$B$4:$I$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Equipment - budzet'!$B$4:$I$35</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -64,12 +64,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="O53" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kampen, Jan-Joris van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Contributions of third parties to be budgeted as personell costs or other direct costs. No indirect costs on these costs when NOT used on the premises of the benificiary.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="105">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -368,7 +392,22 @@
     <t>WP9- Evaluacija I disiminacija</t>
   </si>
   <si>
-    <t>133360</t>
+    <t>70800</t>
+  </si>
+  <si>
+    <t>2S-2G</t>
+  </si>
+  <si>
+    <t>non-profit</t>
+  </si>
+  <si>
+    <t>TomTom NL</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>22720</t>
   </si>
 </sst>
 </file>
@@ -740,7 +779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -844,48 +883,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -906,22 +916,77 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1018,6 +1083,75 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="841473" cy="885911"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="108857" y="519765"/>
+          <a:ext cx="841473" cy="885911"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1311,10 +1445,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T40"/>
+  <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="85" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74:P74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1339,65 +1473,71 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D4" s="2"/>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="3"/>
-      <c r="L4" s="66" t="s">
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D5" s="2"/>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="3"/>
-      <c r="L5" s="66" t="s">
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D6" s="2"/>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="3"/>
-      <c r="L6" s="66" t="s">
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1407,19 +1547,21 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="3"/>
-      <c r="L7" s="66" t="s">
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L7" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1430,56 +1572,56 @@
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="68"/>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="68"/>
-      <c r="R10" s="68"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="70" t="s">
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="70"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="70"/>
-      <c r="P12" s="70"/>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="70"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="47" t="s">
         <v>61</v>
       </c>
@@ -1530,99 +1672,93 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
       <c r="D14" s="15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="15">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H14" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I14" s="16">
         <f>+SUM(D14:H14)</f>
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J14" s="17">
-        <v>60600</v>
-      </c>
-      <c r="K14" s="74">
-        <v>160466</v>
+        <v>39600</v>
+      </c>
+      <c r="K14" s="53">
+        <v>135800</v>
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
       <c r="O14" s="18">
         <f>+$O$4*(J14+K14-N14)</f>
-        <v>55266.5</v>
+        <v>43850</v>
       </c>
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f>+J14+K14+L14+M14+O14+P14</f>
-        <v>276332.5</v>
+        <v>219250</v>
       </c>
       <c r="R14" s="18"/>
       <c r="S14" s="18">
         <f>+Q14-R14</f>
-        <v>276332.5</v>
+        <v>219250</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="15">
-        <v>2</v>
-      </c>
-      <c r="E15" s="15">
-        <v>3</v>
-      </c>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="16">
         <f t="shared" ref="I15:I23" si="0">+SUM(D15:H15)</f>
-        <v>5</v>
-      </c>
-      <c r="J15" s="17">
-        <v>7500</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="18">
         <f t="shared" ref="O15:O23" si="1">+$O$4*(J15+K15-N15)</f>
-        <v>1875</v>
+        <v>0</v>
       </c>
       <c r="P15" s="17"/>
       <c r="Q15" s="17">
         <f t="shared" ref="Q15:Q23" si="2">+J15+K15+L15+M15+O15+P15</f>
-        <v>9375</v>
+        <v>0</v>
       </c>
       <c r="R15" s="18"/>
       <c r="S15" s="18">
         <f t="shared" ref="S15:S23" si="3">+Q15-R15</f>
-        <v>9375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="15">
         <v>2</v>
       </c>
@@ -1663,59 +1799,55 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15">
-        <v>3</v>
-      </c>
-      <c r="F17" s="15">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J17" s="17">
-        <v>16450</v>
-      </c>
-      <c r="K17" s="17">
-        <v>38570</v>
-      </c>
+        <v>1650</v>
+      </c>
+      <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="18">
         <f t="shared" si="1"/>
-        <v>13755</v>
+        <v>412.5</v>
       </c>
       <c r="P17" s="17"/>
       <c r="Q17" s="17">
         <f t="shared" si="2"/>
-        <v>68775</v>
+        <v>2062.5</v>
       </c>
       <c r="R17" s="18"/>
       <c r="S17" s="18">
         <f t="shared" si="3"/>
-        <v>68775</v>
+        <v>2062.5</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="15">
         <v>2</v>
       </c>
       <c r="E18" s="15">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F18" s="15">
         <v>2</v>
@@ -1728,85 +1860,79 @@
       </c>
       <c r="I18" s="16">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J18" s="17">
-        <v>60900</v>
-      </c>
-      <c r="K18" s="17">
-        <v>19924</v>
-      </c>
+        <v>42900</v>
+      </c>
+      <c r="K18" s="17"/>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="18">
         <f t="shared" si="1"/>
-        <v>20206</v>
+        <v>10725</v>
       </c>
       <c r="P18" s="17"/>
       <c r="Q18" s="17">
         <f t="shared" si="2"/>
-        <v>101030</v>
+        <v>53625</v>
       </c>
       <c r="R18" s="18"/>
       <c r="S18" s="18">
         <f t="shared" si="3"/>
-        <v>101030</v>
+        <v>53625</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F19" s="15">
         <v>1</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J19" s="17">
-        <v>47250</v>
-      </c>
-      <c r="K19" s="17">
-        <v>55370</v>
-      </c>
-      <c r="L19" s="17">
-        <v>5000</v>
-      </c>
+        <v>8250</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="18">
         <f>+$O$4*(J19+K19-N19)</f>
-        <v>25655</v>
+        <v>2062.5</v>
       </c>
       <c r="P19" s="17"/>
       <c r="Q19" s="17">
         <f>+J19+K19+L19+M19+O19+P19</f>
-        <v>133275</v>
+        <v>10312.5</v>
       </c>
       <c r="R19" s="18"/>
       <c r="S19" s="18">
         <f t="shared" si="3"/>
-        <v>133275</v>
+        <v>10312.5</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15">
         <v>12</v>
@@ -1845,11 +1971,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
       <c r="D21" s="15">
         <v>3</v>
       </c>
@@ -1886,58 +2012,56 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
       <c r="D22" s="15">
         <v>1</v>
       </c>
       <c r="E22" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I22" s="16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J22" s="17">
-        <v>15900</v>
-      </c>
-      <c r="K22" s="17">
-        <v>3334</v>
-      </c>
+        <v>9900</v>
+      </c>
+      <c r="K22" s="17"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="18">
         <f t="shared" si="1"/>
-        <v>4808.5</v>
+        <v>2475</v>
       </c>
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="2"/>
-        <v>24042.5</v>
+        <v>12375</v>
       </c>
       <c r="R22" s="18"/>
       <c r="S22" s="18">
         <f t="shared" si="3"/>
-        <v>24042.5</v>
+        <v>12375</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -1968,46 +2092,46 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" s="62" t="s">
+      <c r="A24" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E24" s="15">
         <f t="shared" ref="E24:I24" si="4">SUM(E14:E23)</f>
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G24" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H24" s="15">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I24" s="19">
         <f t="shared" si="4"/>
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="J24" s="20">
         <f>SUM(J14:J23)</f>
-        <v>282850</v>
+        <v>176550</v>
       </c>
       <c r="K24" s="20">
         <f>SUM(K14:K23)</f>
-        <v>277664</v>
+        <v>135800</v>
       </c>
       <c r="L24" s="20">
         <f t="shared" ref="L24:S24" si="5">SUM(L14:L23)</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M24" s="20">
         <f t="shared" si="5"/>
@@ -2019,7 +2143,7 @@
       </c>
       <c r="O24" s="20">
         <f t="shared" si="5"/>
-        <v>140128.5</v>
+        <v>78087.5</v>
       </c>
       <c r="P24" s="20">
         <f t="shared" si="5"/>
@@ -2027,7 +2151,7 @@
       </c>
       <c r="Q24" s="20">
         <f t="shared" si="5"/>
-        <v>705642.5</v>
+        <v>390437.5</v>
       </c>
       <c r="R24" s="21">
         <f t="shared" si="5"/>
@@ -2035,7 +2159,7 @@
       </c>
       <c r="S24" s="22">
         <f t="shared" si="5"/>
-        <v>705642.5</v>
+        <v>390437.5</v>
       </c>
       <c r="T24" s="23"/>
     </row>
@@ -2075,7 +2199,7 @@
       <c r="I26" s="29"/>
       <c r="J26" s="20">
         <f>IF(I24=0,0,(J24/I24))</f>
-        <v>1824.8387096774193</v>
+        <v>1650</v>
       </c>
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
@@ -2093,24 +2217,24 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="32"/>
@@ -2151,101 +2275,99 @@
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="54" t="str">
+      <c r="A31" s="65" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
-        <v xml:space="preserve">participant </v>
-      </c>
-      <c r="B31" s="55"/>
+        <v>participant ETF</v>
+      </c>
+      <c r="B31" s="66"/>
       <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="58" t="s">
+      <c r="D31" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59"/>
-      <c r="N31" s="59"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
     </row>
     <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="73" t="s">
+      <c r="B32" s="68"/>
+      <c r="C32" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="53"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="53"/>
-      <c r="P32" s="53"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="70"/>
+      <c r="N32" s="70"/>
+      <c r="O32" s="70"/>
+      <c r="P32" s="70"/>
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="48"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="34">
-        <v>111804</v>
-      </c>
-      <c r="D33" s="53" t="s">
+        <v>65000</v>
+      </c>
+      <c r="D33" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="53"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="70"/>
+      <c r="P33" s="70"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="48"/>
-      <c r="C34" s="34">
-        <v>32500</v>
-      </c>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="53"/>
-      <c r="N34" s="53"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -2279,106 +2401,1155 @@
       <c r="P36" s="37"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A37" s="54" t="str">
+      <c r="A37" s="65" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="55"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="56" t="s">
+      <c r="D37" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="57"/>
-      <c r="M37" s="57"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="57"/>
-      <c r="P37" s="57"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="76"/>
+      <c r="O37" s="76"/>
+      <c r="P37" s="76"/>
     </row>
     <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="48"/>
-      <c r="C38" s="34">
-        <v>5000</v>
-      </c>
-      <c r="D38" s="52" t="s">
+      <c r="B38" s="68"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
-      <c r="O38" s="53"/>
-      <c r="P38" s="53"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="70"/>
+      <c r="N38" s="70"/>
+      <c r="O38" s="70"/>
+      <c r="P38" s="70"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="48"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="34"/>
-      <c r="D39" s="49" t="s">
+      <c r="D39" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="51"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="72"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="72"/>
+      <c r="O39" s="72"/>
+      <c r="P39" s="73"/>
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="48"/>
+      <c r="B40" s="68"/>
       <c r="C40" s="34"/>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
-      <c r="O40" s="53"/>
-      <c r="P40" s="53"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="70"/>
+      <c r="N40" s="70"/>
+      <c r="O40" s="70"/>
+      <c r="P40" s="70"/>
       <c r="S40" s="31"/>
+    </row>
+    <row r="41" spans="1:19" ht="25" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D44" s="2"/>
+      <c r="E44" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="L44" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="M44" s="57"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D45" s="2"/>
+      <c r="E45" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="L45" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="M45" s="57"/>
+      <c r="N45" s="57"/>
+      <c r="O45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D46" s="2"/>
+      <c r="E46" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="L46" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q46" s="6"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="E47" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="L47" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="J48" s="2"/>
+      <c r="O48" s="7"/>
+    </row>
+    <row r="49" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="50" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="59"/>
+      <c r="J50" s="59"/>
+      <c r="K50" s="59"/>
+      <c r="L50" s="59"/>
+      <c r="M50" s="59"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="59"/>
+      <c r="P50" s="59"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="8"/>
+    </row>
+    <row r="52" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D52" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="60"/>
+      <c r="J52" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="61"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="61"/>
+      <c r="N52" s="61"/>
+      <c r="O52" s="61"/>
+      <c r="P52" s="61"/>
+      <c r="Q52" s="61"/>
+      <c r="R52" s="61"/>
+      <c r="S52" s="9"/>
+    </row>
+    <row r="53" spans="1:19" ht="78" x14ac:dyDescent="0.35">
+      <c r="A53" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="54"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J53" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="L53" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N53" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="O53" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P53" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q53" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="R53" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S53" s="48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A54" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="63"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="16">
+        <f>+SUM(D54:H54)</f>
+        <v>0</v>
+      </c>
+      <c r="J54" s="17"/>
+      <c r="K54" s="53"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="18">
+        <f>+$O$4*(J54+K54-N54)</f>
+        <v>0</v>
+      </c>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17">
+        <f>+J54+K54+L54+M54+O54+P54</f>
+        <v>0</v>
+      </c>
+      <c r="R54" s="18"/>
+      <c r="S54" s="18">
+        <f>+Q54-R54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A55" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="63"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="16">
+        <f t="shared" ref="I55:I63" si="6">+SUM(D55:H55)</f>
+        <v>0</v>
+      </c>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="18">
+        <f t="shared" ref="O55:O63" si="7">+$O$4*(J55+K55-N55)</f>
+        <v>0</v>
+      </c>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17">
+        <f t="shared" ref="Q55:Q63" si="8">+J55+K55+L55+M55+O55+P55</f>
+        <v>0</v>
+      </c>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18">
+        <f t="shared" ref="S55:S63" si="9">+Q55-R55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A56" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="63"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A57" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="63"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15">
+        <v>1</v>
+      </c>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J57" s="17">
+        <v>3800</v>
+      </c>
+      <c r="K57" s="17">
+        <v>8010</v>
+      </c>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="18">
+        <f t="shared" si="7"/>
+        <v>2952.5</v>
+      </c>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17">
+        <f t="shared" si="8"/>
+        <v>14762.5</v>
+      </c>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18">
+        <f t="shared" si="9"/>
+        <v>14762.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A58" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R58" s="18"/>
+      <c r="S58" s="18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A59" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="63"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15">
+        <v>3</v>
+      </c>
+      <c r="F59" s="15">
+        <v>1</v>
+      </c>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15">
+        <v>1</v>
+      </c>
+      <c r="I59" s="16">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="J59" s="17">
+        <v>19000</v>
+      </c>
+      <c r="K59" s="17">
+        <v>30010</v>
+      </c>
+      <c r="L59" s="17">
+        <v>2000</v>
+      </c>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="18">
+        <f>+$O$4*(J59+K59-N59)</f>
+        <v>12252.5</v>
+      </c>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17">
+        <f>+J59+K59+L59+M59+O59+P59</f>
+        <v>63262.5</v>
+      </c>
+      <c r="R59" s="18"/>
+      <c r="S59" s="18">
+        <f t="shared" si="9"/>
+        <v>63262.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A60" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="63"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="17"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="18">
+        <f t="shared" ref="O60:O68" si="10">+$O$4*(J60+K60-N60)</f>
+        <v>0</v>
+      </c>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="17">
+        <f t="shared" ref="Q60:Q68" si="11">+J60+K60+L60+M60+O60+P60</f>
+        <v>0</v>
+      </c>
+      <c r="R60" s="18"/>
+      <c r="S60" s="18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A61" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="63"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="17"/>
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P61" s="17"/>
+      <c r="Q61" s="17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A62" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="63"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R62" s="18"/>
+      <c r="S62" s="18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A63" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="63"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R63" s="18"/>
+      <c r="S63" s="18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A64" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="64"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="15">
+        <f>SUM(D54:D63)</f>
+        <v>0</v>
+      </c>
+      <c r="E64" s="15">
+        <f t="shared" ref="E64:I64" si="12">SUM(E54:E63)</f>
+        <v>4</v>
+      </c>
+      <c r="F64" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="G64" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="H64" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="I64" s="19">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="J64" s="20">
+        <f>SUM(J54:J63)</f>
+        <v>22800</v>
+      </c>
+      <c r="K64" s="20">
+        <f>SUM(K54:K63)</f>
+        <v>38020</v>
+      </c>
+      <c r="L64" s="20">
+        <f t="shared" ref="L64:S64" si="13">SUM(L54:L63)</f>
+        <v>2000</v>
+      </c>
+      <c r="M64" s="20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="N64" s="20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O64" s="20">
+        <f t="shared" si="13"/>
+        <v>15205</v>
+      </c>
+      <c r="P64" s="20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q64" s="20">
+        <f t="shared" si="13"/>
+        <v>78025</v>
+      </c>
+      <c r="R64" s="21">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S64" s="22">
+        <f t="shared" si="13"/>
+        <v>78025</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A65" s="24"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="23"/>
+      <c r="N65" s="23"/>
+      <c r="O65" s="23"/>
+      <c r="P65" s="23"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="23"/>
+      <c r="S65" s="23"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A66" s="24"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E66" s="27"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="20">
+        <f>IF(I64=0,0,(J64/I64))</f>
+        <v>3800</v>
+      </c>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="23"/>
+      <c r="N66" s="23"/>
+      <c r="O66" s="23"/>
+      <c r="P66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="23"/>
+      <c r="S66" s="23"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A67" s="30"/>
+      <c r="S67" s="31"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A68" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="62"/>
+      <c r="F68" s="62"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="62"/>
+      <c r="I68" s="62"/>
+      <c r="J68" s="62"/>
+      <c r="K68" s="62"/>
+      <c r="L68" s="62"/>
+      <c r="M68" s="62"/>
+      <c r="N68" s="62"/>
+      <c r="O68" s="62"/>
+      <c r="P68" s="62"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A69" s="50"/>
+      <c r="B69" s="50"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="50"/>
+      <c r="H69" s="50"/>
+      <c r="I69" s="50"/>
+      <c r="J69" s="50"/>
+      <c r="K69" s="50"/>
+      <c r="L69" s="50"/>
+      <c r="M69" s="50"/>
+      <c r="N69" s="50"/>
+      <c r="O69" s="50"/>
+      <c r="P69" s="50"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A70" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="50"/>
+      <c r="K70" s="50"/>
+      <c r="L70" s="50"/>
+      <c r="M70" s="50"/>
+      <c r="N70" s="50"/>
+      <c r="O70" s="50"/>
+      <c r="P70" s="50"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A71" s="65" t="str">
+        <f>CONCATENATE("participant"," ",J46)</f>
+        <v>participant TOM</v>
+      </c>
+      <c r="B71" s="66"/>
+      <c r="C71" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="67"/>
+      <c r="F71" s="67"/>
+      <c r="G71" s="67"/>
+      <c r="H71" s="67"/>
+      <c r="I71" s="67"/>
+      <c r="J71" s="67"/>
+      <c r="K71" s="67"/>
+      <c r="L71" s="67"/>
+      <c r="M71" s="67"/>
+      <c r="N71" s="67"/>
+      <c r="O71" s="67"/>
+      <c r="P71" s="67"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A72" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="68"/>
+      <c r="C72" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D72" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="E72" s="70"/>
+      <c r="F72" s="70"/>
+      <c r="G72" s="70"/>
+      <c r="H72" s="70"/>
+      <c r="I72" s="70"/>
+      <c r="J72" s="70"/>
+      <c r="K72" s="70"/>
+      <c r="L72" s="70"/>
+      <c r="M72" s="70"/>
+      <c r="N72" s="70"/>
+      <c r="O72" s="70"/>
+      <c r="P72" s="70"/>
+      <c r="S72" s="31"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A73" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" s="68"/>
+      <c r="C73" s="34">
+        <v>7800</v>
+      </c>
+      <c r="D73" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="E73" s="70"/>
+      <c r="F73" s="70"/>
+      <c r="G73" s="70"/>
+      <c r="H73" s="70"/>
+      <c r="I73" s="70"/>
+      <c r="J73" s="70"/>
+      <c r="K73" s="70"/>
+      <c r="L73" s="70"/>
+      <c r="M73" s="70"/>
+      <c r="N73" s="70"/>
+      <c r="O73" s="70"/>
+      <c r="P73" s="70"/>
+      <c r="S73" s="31"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A74" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" s="68"/>
+      <c r="C74" s="34">
+        <v>7500</v>
+      </c>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
+      <c r="F74" s="70"/>
+      <c r="G74" s="70"/>
+      <c r="H74" s="70"/>
+      <c r="I74" s="70"/>
+      <c r="J74" s="70"/>
+      <c r="K74" s="70"/>
+      <c r="L74" s="70"/>
+      <c r="M74" s="70"/>
+      <c r="N74" s="70"/>
+      <c r="O74" s="70"/>
+      <c r="P74" s="70"/>
+      <c r="S74" s="31"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A75" s="35"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="36"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
+      <c r="L75" s="36"/>
+      <c r="M75" s="36"/>
+      <c r="N75" s="36"/>
+      <c r="O75" s="36"/>
+      <c r="P75" s="36"/>
+      <c r="Q75" s="35"/>
+      <c r="R75" s="35"/>
+      <c r="S75" s="35"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="37"/>
+      <c r="K76" s="37"/>
+      <c r="L76" s="37"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="37"/>
+      <c r="O76" s="37"/>
+      <c r="P76" s="37"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A77" s="65" t="str">
+        <f>CONCATENATE("participant"," ",C49)</f>
+        <v xml:space="preserve">participant </v>
+      </c>
+      <c r="B77" s="66"/>
+      <c r="C77" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D77" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="76"/>
+      <c r="F77" s="76"/>
+      <c r="G77" s="76"/>
+      <c r="H77" s="76"/>
+      <c r="I77" s="76"/>
+      <c r="J77" s="76"/>
+      <c r="K77" s="76"/>
+      <c r="L77" s="76"/>
+      <c r="M77" s="76"/>
+      <c r="N77" s="76"/>
+      <c r="O77" s="76"/>
+      <c r="P77" s="76"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A78" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="68"/>
+      <c r="C78" s="34">
+        <v>2000</v>
+      </c>
+      <c r="D78" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78" s="70"/>
+      <c r="F78" s="70"/>
+      <c r="G78" s="70"/>
+      <c r="H78" s="70"/>
+      <c r="I78" s="70"/>
+      <c r="J78" s="70"/>
+      <c r="K78" s="70"/>
+      <c r="L78" s="70"/>
+      <c r="M78" s="70"/>
+      <c r="N78" s="70"/>
+      <c r="O78" s="70"/>
+      <c r="P78" s="70"/>
+      <c r="S78" s="31"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A79" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B79" s="68"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="E79" s="72"/>
+      <c r="F79" s="72"/>
+      <c r="G79" s="72"/>
+      <c r="H79" s="72"/>
+      <c r="I79" s="72"/>
+      <c r="J79" s="72"/>
+      <c r="K79" s="72"/>
+      <c r="L79" s="72"/>
+      <c r="M79" s="72"/>
+      <c r="N79" s="72"/>
+      <c r="O79" s="72"/>
+      <c r="P79" s="73"/>
+      <c r="S79" s="31"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A80" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="B80" s="68"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="E80" s="70"/>
+      <c r="F80" s="70"/>
+      <c r="G80" s="70"/>
+      <c r="H80" s="70"/>
+      <c r="I80" s="70"/>
+      <c r="J80" s="70"/>
+      <c r="K80" s="70"/>
+      <c r="L80" s="70"/>
+      <c r="M80" s="70"/>
+      <c r="N80" s="70"/>
+      <c r="O80" s="70"/>
+      <c r="P80" s="70"/>
+      <c r="S80" s="31"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="C32:P40 D14:H23 P14:P23 R14:S23 O6 J14:J23 L14:N23 K15:K23" name="Range1"/>
+    <protectedRange sqref="C32:P40 D14:H23 P14:P23 R14:S23 O6 J14:J23 L14:N23 K15:K23 C72:P80 D54:H63 P54:P63 R54:S63 O46 J54:J63 L54:N63 K55:K63" name="Range1"/>
   </protectedRanges>
-  <mergeCells count="41">
+  <mergeCells count="82">
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="D78:P78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:P79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:P80"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:P73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:P74"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="D77:P77"/>
+    <mergeCell ref="A68:P68"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:P71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:P72"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A50:R50"/>
+    <mergeCell ref="D52:I52"/>
+    <mergeCell ref="J52:R52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:P39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:P40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:P34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E4:I4"/>
@@ -2392,42 +3563,19 @@
     <mergeCell ref="A10:R10"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="J12:R12"/>
-    <mergeCell ref="A28:P28"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:P39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:P40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND($O$4="",$G$7="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O44">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($O$4="",$G$7="")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6 O46">
       <formula1>"70%, 100%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2443,7 +3591,7 @@
   <dimension ref="B1:P35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2457,10 +3605,10 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:16" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="72"/>
+      <c r="C2" s="78"/>
       <c r="D2" s="42">
         <f>SUM(P5:P35)</f>
         <v>133360</v>
@@ -3330,8 +4478,502 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="87" customWidth="1"/>
+    <col min="7" max="7" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="42">
+        <f>SUM(I5:I35)</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="38">
+        <v>3000</v>
+      </c>
+      <c r="H5" s="38">
+        <v>1</v>
+      </c>
+      <c r="I5" s="38">
+        <f>G5*H5</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="38">
+        <v>2000</v>
+      </c>
+      <c r="H6" s="38">
+        <v>1</v>
+      </c>
+      <c r="I6" s="38">
+        <f t="shared" ref="I6:I35" si="0">G6*H6</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I35"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3347,10 +4989,10 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="72"/>
+      <c r="C2" s="78"/>
       <c r="D2" s="42">
         <f>SUM(I5:I35)</f>
         <v>111804</v>
@@ -3567,7 +5209,7 @@
         <v>4</v>
       </c>
       <c r="I11" s="38">
-        <f t="shared" si="0"/>
+        <f>G11*H11</f>
         <v>5204</v>
       </c>
     </row>
@@ -3918,498 +5560,4 @@
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="87" customWidth="1"/>
-    <col min="7" max="7" width="34.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="42">
-        <f>SUM(I5:I35)</f>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="38">
-        <v>3000</v>
-      </c>
-      <c r="H5" s="38">
-        <v>1</v>
-      </c>
-      <c r="I5" s="38">
-        <f>G5*H5</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="38">
-        <v>2000</v>
-      </c>
-      <c r="H6" s="38">
-        <v>1</v>
-      </c>
-      <c r="I6" s="38">
-        <f t="shared" ref="I6:I35" si="0">G6*H6</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>